<commit_message>
Dodate i ostale lokacije
</commit_message>
<xml_diff>
--- a/samoPouzdaniPodaciTabela.xlsx
+++ b/samoPouzdaniPodaciTabela.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13080"/>
+    <workbookView windowWidth="23970" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>ams</t>
   </si>
@@ -101,6 +101,48 @@
   </si>
   <si>
     <t>Jabuka</t>
+  </si>
+  <si>
+    <t>00000EA1</t>
+  </si>
+  <si>
+    <t>Zrenjanin</t>
+  </si>
+  <si>
+    <t>Sutjeska</t>
+  </si>
+  <si>
+    <t>07.12.2011</t>
+  </si>
+  <si>
+    <t>Sljiva</t>
+  </si>
+  <si>
+    <t>00000DAD</t>
+  </si>
+  <si>
+    <t>Kikinda</t>
+  </si>
+  <si>
+    <t>12.03.2012</t>
+  </si>
+  <si>
+    <t>Od 28.06.2018. kisomer ne meri kolicinu padavina  10.07.2018.skinut je kisomer koji ne meri kolicinu padavina i sutra ide u Suboticu na servis.Kisomer je postavljen sa novim senzorom za merenje količine padavina 17.07.</t>
+  </si>
+  <si>
+    <t>00000E8C</t>
+  </si>
+  <si>
+    <t>Nestin</t>
+  </si>
+  <si>
+    <t>01.10.2012</t>
+  </si>
+  <si>
+    <t>Kruska</t>
+  </si>
+  <si>
+    <t>Bila je pre toga jabuka - zabelezi !!!</t>
   </si>
 </sst>
 </file>
@@ -108,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -146,7 +188,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,6 +203,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -168,36 +233,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -206,6 +241,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -217,65 +318,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,43 +332,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,139 +506,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,6 +533,36 @@
       </top>
       <bottom style="thin">
         <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,17 +585,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,182 +634,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1081,13 +1123,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="30.7" customWidth="1"/>
     <col min="3" max="3" width="22.9" customWidth="1"/>
@@ -1212,6 +1254,63 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>